<commit_message>
updated template to fix formatting
</commit_message>
<xml_diff>
--- a/data_inventory_template.xlsx
+++ b/data_inventory_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/grete_graf_yale_edu/Documents/Documents/DP_data_inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{31DBF1F8-720A-4295-A04D-DDF0240DF004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2844CC36-20BF-4D61-B0B6-2A5D96C74D28}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{31DBF1F8-720A-4295-A04D-DDF0240DF004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD2C379B-3FC6-4F4C-A62F-1109F2B7E773}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -408,7 +408,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,13 +418,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -583,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -636,6 +629,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -650,22 +652,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,171 +945,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B0BAC4-74A0-40CE-BE89-F793B08C9CC7}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="100.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.140625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="35"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="34"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="34"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34" t="s">
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34" t="s">
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34" t="s">
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34" t="s">
+    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+    <row r="17" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+    <row r="18" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+    <row r="19" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+    <row r="20" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34" t="s">
+    <row r="22" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="35"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
-      <c r="B24" s="35"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="35"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="35"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="35"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="38"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="38"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="38"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="38"/>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="29"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="30"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="30"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="30"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1135,9 +1084,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C512A8CD-50ED-4313-BDF0-EFEFD82F3C46}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1097,7 @@
     <col min="4" max="4" width="154.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>62</v>
       </c>
@@ -1159,8 +1108,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -1173,8 +1122,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
@@ -1183,8 +1132,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
         <v>1</v>
@@ -1193,8 +1142,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
         <v>2</v>
@@ -1203,8 +1152,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
       <c r="B6" s="6" t="s">
         <v>58</v>
       </c>
@@ -1215,8 +1164,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
         <v>39</v>
@@ -1225,8 +1174,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>12</v>
@@ -1235,8 +1184,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>10</v>
@@ -1245,8 +1194,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>11</v>
@@ -1255,8 +1204,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
       <c r="B11" s="8" t="s">
         <v>59</v>
       </c>
@@ -1267,8 +1216,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
+    <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14" t="s">
         <v>7</v>
@@ -1277,8 +1226,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
         <v>56</v>
       </c>
       <c r="B13" s="8"/>
@@ -1289,8 +1238,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
         <v>4</v>
@@ -1299,8 +1248,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
         <v>19</v>
@@ -1309,8 +1258,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
         <v>18</v>
@@ -1319,8 +1268,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
       <c r="B17" s="9" t="s">
         <v>63</v>
       </c>
@@ -1331,8 +1280,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
         <v>35</v>
@@ -1341,8 +1290,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9" t="s">
         <v>14</v>
@@ -1351,8 +1300,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9" t="s">
         <v>17</v>
@@ -1361,8 +1310,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
         <v>33</v>
@@ -1371,8 +1320,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
       <c r="B22" s="10" t="s">
         <v>61</v>
       </c>
@@ -1383,8 +1332,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
         <v>36</v>
@@ -1393,8 +1342,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
         <v>13</v>
@@ -1403,8 +1352,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
         <v>15</v>
@@ -1413,8 +1362,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+    <row r="26" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="33"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18" t="s">
         <v>8</v>
@@ -1471,72 +1420,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32" t="s">
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32" t="s">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>